<commit_message>
PHAST files are updated with 'folder' for 'E-B-;
</commit_message>
<xml_diff>
--- a/H2495_FRA/H2495_c.xlsx
+++ b/H2495_FRA/H2495_c.xlsx
@@ -6,10 +6,10 @@
     <x:workbookView activeTab="3"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Discharge" sheetId="2" r:id="R015764f8c4d84159"/>
-    <x:sheet name="Flammable Dispersion" sheetId="3" r:id="Rc4e374bbd8964f78"/>
-    <x:sheet name="Jet fire" sheetId="4" r:id="R3793b70d25844d2e"/>
-    <x:sheet name="Explosions" sheetId="5" r:id="Rbb82dbcfeb7b4fff"/>
+    <x:sheet name="Discharge" sheetId="2" r:id="R74c91c5f58154784"/>
+    <x:sheet name="Flammable Dispersion" sheetId="3" r:id="R15a7b82f1bf141a6"/>
+    <x:sheet name="Jet fire" sheetId="4" r:id="R2ee559966fca42ae"/>
+    <x:sheet name="Explosions" sheetId="5" r:id="Rdb6bc6f42e6a458e"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -62,7 +62,7 @@
     <x:t>Droplet diameter (um)</x:t>
   </x:si>
   <x:si>
-    <x:t>H2495\S3</x:t>
+    <x:t>H2495\S3\EOBO</x:t>
   </x:si>
   <x:si>
     <x:t>SM</x:t>
@@ -83,10 +83,10 @@
     <x:t>LA</x:t>
   </x:si>
   <x:si>
-    <x:t>H2495\S8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>H2495\S9</x:t>
+    <x:t>H2495\S8\EOBO</x:t>
+  </x:si>
+  <x:si>
+    <x:t>H2495\S9\EOBN</x:t>
   </x:si>
   <x:si>
     <x:t>Averaging time (s)</x:t>

</xml_diff>